<commit_message>
Fixed population data type and added report #5
</commit_message>
<xml_diff>
--- a/IT410 Final Project/Data/Population Per Country.xlsx
+++ b/IT410 Final Project/Data/Population Per Country.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\IT410 Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FE088D-9CFE-4F94-9D97-BA6FE5D0AA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4A1521-89E7-4091-B4A9-0D69058BFB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10176" yWindow="2796" windowWidth="10608" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23112" windowHeight="11292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -10197,7 +10197,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10539,8 +10539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A595" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D602" sqref="D602"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>